<commit_message>
Visuals for q1, q2
</commit_message>
<xml_diff>
--- a/notebook/cluster_results_cleaned.xlsx
+++ b/notebook/cluster_results_cleaned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iason\OneDrive\Υπολογιστής\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9E2675-9700-498A-B7C7-60B3DB330992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D763AE-FB3A-4861-9539-C8153B1B1687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{32966D09-A2B0-49AE-A46C-FB656EA3DAEA}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{32966D09-A2B0-49AE-A46C-FB656EA3DAEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
   <si>
     <t>cluster</t>
   </si>
@@ -101,24 +101,12 @@
     <t>ΕΒΑΠΟΡΕ</t>
   </si>
   <si>
-    <t>ΚΟΚΚΙΝΟ</t>
-  </si>
-  <si>
     <t>COLA</t>
   </si>
   <si>
-    <t>ΠΡΑΛΙΝΕΣ SPREADS</t>
-  </si>
-  <si>
     <t>WAFER</t>
   </si>
   <si>
-    <t>ΕΝΕΡΓΕΙΑΚΑ ΙΣΟΤΟΝΙΚΑ</t>
-  </si>
-  <si>
-    <t>ΜΠΥΡΕΣ ΦΙΑΛΗ</t>
-  </si>
-  <si>
     <t>ΓΑΤΑ</t>
   </si>
   <si>
@@ -131,9 +119,6 @@
     <t>ΛΕΜΟΝΑΔΑ</t>
   </si>
   <si>
-    <t>ΟΥΖΟ</t>
-  </si>
-  <si>
     <t>ΓΑΛΑΤΑ</t>
   </si>
   <si>
@@ -155,12 +140,6 @@
     <t>ΚΡΟΥΑΣΑΝ</t>
   </si>
   <si>
-    <t>ΤΥΡΟΚΟΜΙΚΑ</t>
-  </si>
-  <si>
-    <t>ΑΛΛΑΝΤΙΚΑ</t>
-  </si>
-  <si>
     <t>ΒΟΥΤΥΡΑ</t>
   </si>
   <si>
@@ -170,10 +149,82 @@
     <t>ΑΛΕΥΡΙ</t>
   </si>
   <si>
-    <t>ΜΑΛ/ΚΑ ΠΛΥ/ΟΥ</t>
-  </si>
-  <si>
-    <t>ΥΓΡΑ ΜΑΓ/ΚΩΝ ΣΚΕΥΩΝ</t>
+    <t>ΚΡΕΑΣ</t>
+  </si>
+  <si>
+    <t>ΑΥΓΑ</t>
+  </si>
+  <si>
+    <t>ΧΑΡΤΟΠΕΤΣΕΤΕΣ</t>
+  </si>
+  <si>
+    <t>ΛΑΧΑΝΙΚΑ</t>
+  </si>
+  <si>
+    <t>ΚΟΥΖΙΝΑΣ</t>
+  </si>
+  <si>
+    <t>ΖΥΜΕΣ</t>
+  </si>
+  <si>
+    <t>ΥΓΡΑ ΜΑΓΕΙΡΙΚΩΝ ΣΚΕΥΩΝ</t>
+  </si>
+  <si>
+    <t>ΜΑΛΑΚΤΙΚΑ ΠΛΥΝΤΗΡΙΟΥ</t>
+  </si>
+  <si>
+    <t>ΦΥΣΙΚΟΙ</t>
+  </si>
+  <si>
+    <t>ΜΠΥΡΕΣ ΚΟΥΤΙ</t>
+  </si>
+  <si>
+    <t>ΕΛΛΗΝΙΚΑ ΚΡΑΣΙΑ</t>
+  </si>
+  <si>
+    <t>ΜΕΤΑΛΛΙΚΟ</t>
+  </si>
+  <si>
+    <t>ΟΔΟΝΤΟΠΑΣΤΕΣ</t>
+  </si>
+  <si>
+    <t>ΣΑΜΠΟΥΑΝ</t>
+  </si>
+  <si>
+    <t>ΝΕΚΤΑΡ</t>
+  </si>
+  <si>
+    <t>ΕΠΙΤΡΑΠΕΖΙΟ</t>
+  </si>
+  <si>
+    <t>ΦΡΟΥΤΟΠΟΤΑ</t>
+  </si>
+  <si>
+    <t>ΔΗΜΗΤΡΙΑΚΑ</t>
+  </si>
+  <si>
+    <t>ΜΑΚΡΙΑ</t>
+  </si>
+  <si>
+    <t>ΦΡΥΓΑΝΙΕΣ</t>
+  </si>
+  <si>
+    <t>ΣΥΜΠΥΚΝΩΜΕΝΑ</t>
+  </si>
+  <si>
+    <t>cluster_2</t>
+  </si>
+  <si>
+    <t>ΤΥΡΟΚΟΜΙΚΑ_ΧΥΜΑ</t>
+  </si>
+  <si>
+    <t>ΤΥΡΟΚΟΜΙΚΑ_ΣΥΣΚ</t>
+  </si>
+  <si>
+    <t>ΑΛΛΑΝΤΙΚΑ_ΣΥΣΚ</t>
+  </si>
+  <si>
+    <t>ΑΛΛΑΝΤΙΚΑ_ΧΥΜΑ</t>
   </si>
 </sst>
 </file>
@@ -225,12 +276,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132250EB-E747-4DB5-914C-3DF0AE31AA50}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A2:A15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,121 +644,121 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
-        <v>2045</v>
+      <c r="B2">
+        <v>32808</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
-        <v>1607</v>
+      <c r="B3">
+        <v>20582</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
-        <v>501</v>
+      <c r="B4">
+        <v>12850</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4">
-        <v>459</v>
+      <c r="B5">
+        <v>11324</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4">
-        <v>377</v>
+      <c r="B6">
+        <v>7064</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="4">
-        <v>323</v>
+      <c r="B7">
+        <v>5450</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="4">
-        <v>263</v>
+      <c r="B8">
+        <v>5005</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="4">
-        <v>130</v>
+      <c r="B9">
+        <v>4772</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="4">
-        <v>109</v>
+      <c r="B10">
+        <v>4487</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="4">
-        <v>98</v>
+      <c r="B11">
+        <v>3826</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="4">
-        <v>97</v>
+      <c r="B12">
+        <v>3519</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="3"/>
@@ -718,11 +768,11 @@
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="4">
-        <v>77</v>
+      <c r="B13">
+        <v>3451</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="3"/>
@@ -732,11 +782,11 @@
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="4">
-        <v>63</v>
+      <c r="B14">
+        <v>3443</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="3"/>
@@ -746,11 +796,11 @@
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="4">
-        <v>57</v>
+      <c r="B15">
+        <v>3415</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="3"/>
@@ -760,11 +810,11 @@
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="4">
-        <v>20582</v>
+      <c r="B16">
+        <v>3061</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="3"/>
@@ -774,11 +824,11 @@
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="4">
-        <v>19269</v>
+      <c r="B17">
+        <v>2941</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="3"/>
@@ -788,11 +838,11 @@
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="4">
-        <v>12850</v>
+      <c r="B18">
+        <v>2651</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="3"/>
@@ -802,11 +852,11 @@
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="4">
-        <v>11889</v>
+      <c r="B19">
+        <v>2099</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="3"/>
@@ -816,11 +866,11 @@
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="4">
-        <v>7599</v>
+      <c r="B20">
+        <v>1748</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="3"/>
@@ -830,11 +880,11 @@
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="4">
-        <v>7249</v>
+      <c r="B21">
+        <v>1378</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="3"/>
@@ -844,11 +894,11 @@
       <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="4">
-        <v>6887</v>
+      <c r="B22">
+        <v>1166</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="3"/>
@@ -858,11 +908,11 @@
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="4">
-        <v>6468</v>
+      <c r="B23">
+        <v>1143</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="3"/>
@@ -872,220 +922,374 @@
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="4">
-        <v>6191</v>
+      <c r="B24">
+        <v>933</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="4">
-        <v>5375</v>
+      <c r="B25">
+        <v>794</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="4">
-        <v>4968</v>
+      <c r="B26">
+        <v>718</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="4">
-        <v>4638</v>
+      <c r="B27">
+        <v>647</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="4">
-        <v>4336</v>
+      <c r="B28">
+        <v>612</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="4">
-        <v>4048</v>
+      <c r="B29">
+        <v>610</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="4">
-        <v>3061</v>
+      <c r="B30">
+        <v>7264</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="4">
-        <v>2941</v>
+      <c r="B31">
+        <v>3952</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="4">
-        <v>2651</v>
+      <c r="B32">
+        <v>2855</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="4">
-        <v>2099</v>
+      <c r="B33">
+        <v>2399</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="4">
-        <v>1748</v>
+      <c r="B34">
+        <v>2384</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="4">
-        <v>1378</v>
+      <c r="B35">
+        <v>2254</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="4">
-        <v>1166</v>
+      <c r="B36">
+        <v>1561</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="4">
-        <v>1143</v>
+      <c r="B37">
+        <v>1504</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="4">
-        <v>933</v>
+      <c r="B38">
+        <v>1394</v>
       </c>
       <c r="C38" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="4">
-        <v>794</v>
+      <c r="B39">
+        <v>1354</v>
       </c>
       <c r="C39" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="4">
-        <v>718</v>
+      <c r="B40">
+        <v>1321</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="4">
-        <v>647</v>
+      <c r="B41">
+        <v>1217</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="4">
-        <v>612</v>
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>1005</v>
       </c>
       <c r="C42" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="4">
-        <v>610</v>
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>959</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44">
+        <v>19271</v>
+      </c>
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45">
+        <v>12159</v>
+      </c>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46">
+        <v>11483</v>
+      </c>
+      <c r="C46" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47">
+        <v>8883</v>
+      </c>
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48">
+        <v>7307</v>
+      </c>
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49">
+        <v>6468</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50">
+        <v>5684</v>
+      </c>
+      <c r="C50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51">
+        <v>4452</v>
+      </c>
+      <c r="C51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52">
+        <v>4058</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53">
+        <v>4048</v>
+      </c>
+      <c r="C53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54">
+        <v>3829</v>
+      </c>
+      <c r="C54" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55">
+        <v>3619</v>
+      </c>
+      <c r="C55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56">
+        <v>3486</v>
+      </c>
+      <c r="C56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57">
+        <v>3295</v>
+      </c>
+      <c r="C57" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>